<commit_message>
Add bio info, images and sample data for bio-master d
</commit_message>
<xml_diff>
--- a/src/Prototypes/hmi/AI/bio_master_C.xlsx
+++ b/src/Prototypes/hmi/AI/bio_master_C.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Q\Documents\uni\Echo-HMI\AI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Q\Documents\uni\Echo\Project-Echo\src\Prototypes\hmi\AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127FFF6A-5E98-472B-9E5E-EA6EC3CE90CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1785924F-1CF4-4057-9181-A1EEE65E520F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="4940" windowWidth="24300" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="1950" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bio_master_D" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="263">
   <si>
     <t>Animal</t>
   </si>
@@ -811,6 +811,24 @@
   </si>
   <si>
     <t>Common Name</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Kuranda Tree Frog</t>
+  </si>
+  <si>
+    <t>Common Name?</t>
+  </si>
+  <si>
+    <t>Peron's Tree Frog</t>
+  </si>
+  <si>
+    <t>Orange Thighed Tree Frog</t>
+  </si>
+  <si>
+    <t>Purple-crowned fairy wren</t>
   </si>
 </sst>
 </file>
@@ -1880,8 +1898,8 @@
   <dimension ref="A1:O83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1893,7 +1911,7 @@
     <col min="5" max="5" width="10.453125" style="17" customWidth="1"/>
     <col min="6" max="6" width="12.453125" style="18" customWidth="1"/>
     <col min="7" max="7" width="10.81640625" style="19" customWidth="1"/>
-    <col min="8" max="8" width="11.54296875" style="20" customWidth="1"/>
+    <col min="8" max="8" width="17.08984375" style="20" customWidth="1"/>
     <col min="9" max="9" width="13.54296875" style="21" customWidth="1"/>
     <col min="10" max="10" width="27.6328125" style="22" customWidth="1"/>
     <col min="11" max="11" width="15.453125" customWidth="1"/>
@@ -1947,6 +1965,9 @@
       <c r="D2" s="10" t="s">
         <v>92</v>
       </c>
+      <c r="E2" s="17" t="s">
+        <v>257</v>
+      </c>
       <c r="L2" s="8" t="e">
         <f>_xlfn.CONCAT(#REF!,A2,#REF!)</f>
         <v>#REF!</v>
@@ -1960,11 +1981,20 @@
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B3" s="24" t="s">
+        <v>258</v>
+      </c>
       <c r="C3" s="9" t="s">
         <v>175</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>93</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>259</v>
       </c>
       <c r="L3" s="8" t="e">
         <f>_xlfn.CONCAT(#REF!,A3,#REF!)</f>
@@ -1979,11 +2009,17 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B4" s="24" t="s">
+        <v>260</v>
+      </c>
       <c r="C4" s="9" t="s">
         <v>176</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>94</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>259</v>
       </c>
       <c r="L4" s="8" t="e">
         <f>_xlfn.CONCAT(#REF!,A4,#REF!)</f>
@@ -2004,6 +2040,9 @@
       <c r="D5" s="10" t="s">
         <v>95</v>
       </c>
+      <c r="H5" s="20" t="s">
+        <v>7</v>
+      </c>
       <c r="L5" s="8" t="e">
         <f>_xlfn.CONCAT(#REF!,A5,#REF!)</f>
         <v>#REF!</v>
@@ -2023,6 +2062,9 @@
       <c r="D6" s="10" t="s">
         <v>96</v>
       </c>
+      <c r="H6" s="20" t="s">
+        <v>7</v>
+      </c>
       <c r="L6" s="8" t="e">
         <f>_xlfn.CONCAT(#REF!,A6,#REF!)</f>
         <v>#REF!</v>
@@ -2036,11 +2078,17 @@
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B7" s="24" t="s">
+        <v>261</v>
+      </c>
       <c r="C7" s="9" t="s">
         <v>179</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>97</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>259</v>
       </c>
       <c r="L7" s="8" t="e">
         <f>_xlfn.CONCAT(#REF!,A7,#REF!)</f>
@@ -2061,6 +2109,9 @@
       <c r="D8" s="10" t="s">
         <v>98</v>
       </c>
+      <c r="H8" s="20" t="s">
+        <v>7</v>
+      </c>
       <c r="L8" s="8" t="e">
         <f>_xlfn.CONCAT(#REF!,A8,#REF!)</f>
         <v>#REF!</v>
@@ -2080,6 +2131,9 @@
       <c r="D9" s="10" t="s">
         <v>99</v>
       </c>
+      <c r="H9" s="20" t="s">
+        <v>7</v>
+      </c>
       <c r="L9" s="8" t="e">
         <f>_xlfn.CONCAT(#REF!,A9,#REF!)</f>
         <v>#REF!</v>
@@ -2099,6 +2153,9 @@
       <c r="D10" s="10" t="s">
         <v>100</v>
       </c>
+      <c r="H10" s="20" t="s">
+        <v>7</v>
+      </c>
       <c r="L10" s="8" t="e">
         <f>_xlfn.CONCAT(#REF!,A10,#REF!)</f>
         <v>#REF!</v>
@@ -2112,11 +2169,17 @@
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B11" s="24" t="s">
+        <v>262</v>
+      </c>
       <c r="C11" s="9" t="s">
         <v>183</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>101</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>259</v>
       </c>
       <c r="L11" s="8" t="e">
         <f>_xlfn.CONCAT(#REF!,A11,#REF!)</f>

</xml_diff>